<commit_message>
New approach to the project, improving method
Starting in Pruebas1 recreating part of Pruebas 2 to read Laliga.com
</commit_message>
<xml_diff>
--- a/Output Liga Femenina.xlsx
+++ b/Output Liga Femenina.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="105">
   <si>
     <t>Team</t>
   </si>
@@ -246,22 +246,22 @@
     <t>46</t>
   </si>
   <si>
+    <t>45</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
     <t>49</t>
   </si>
   <si>
-    <t>['Tenerife', 'Valencia Fem', 'Real Betis Fem', 'Deportivo']</t>
-  </si>
-  <si>
-    <t>['Real Sociedad', 'Valencia Fem', 'Tenerife', 'Sporting Huelva']</t>
-  </si>
-  <si>
-    <t>['Athletic Fem', 'Alhama ElPozo', 'Deportivo', 'Levante Planas']</t>
+    <t>['Levante Planas', 'Tenerife', 'Valencia Fem', 'Real Betis Fem', 'Deportivo']</t>
+  </si>
+  <si>
+    <t>['Athletic Fem', 'Real Sociedad', 'Valencia Fem', 'Tenerife', 'Sporting Huelva']</t>
+  </si>
+  <si>
+    <t>['Tenerife', 'Athletic Fem', 'Alhama ElPozo', 'Deportivo', 'Levante Planas']</t>
   </si>
   <si>
     <t>['Sporting Huelva', 'Athletic Fem']</t>
@@ -270,16 +270,16 @@
     <t>['Real Betis Fem', 'Villarreal']</t>
   </si>
   <si>
-    <t>['Levante Planas', 'Real Betis Fem']</t>
+    <t>['Villarreal', 'Levante Planas', 'Real Betis Fem']</t>
+  </si>
+  <si>
+    <t>['Madrid CFF Fem', 'Sporting Huelva', 'Villarreal', 'Real Sociedad']</t>
   </si>
   <si>
     <t>['Sporting Huelva']</t>
   </si>
   <si>
-    <t>['Sporting Huelva', 'Villarreal', 'Real Sociedad']</t>
-  </si>
-  <si>
-    <t>['Athletic Fem']</t>
+    <t>['Real Sociedad', 'Athletic Fem']</t>
   </si>
   <si>
     <t>[]</t>
@@ -288,19 +288,22 @@
     <t>['Deportivo']</t>
   </si>
   <si>
-    <t>['Real Betis Fem']</t>
+    <t>['Athletic Fem', 'Real Betis Fem']</t>
+  </si>
+  <si>
+    <t>['Sevilla FC Fem']</t>
   </si>
   <si>
     <t>['Barcelona Fem', 'Real Madrid Fem']</t>
   </si>
   <si>
-    <t>['Real Madrid Fem', 'Sevilla FC Fem']</t>
-  </si>
-  <si>
-    <t>['Levante Fem', 'Real Madrid Fem', 'Tenerife', 'AtlÃ©tico Fem']</t>
-  </si>
-  <si>
-    <t>['Real Sociedad', 'Sevilla FC Fem', 'AtlÃ©tico Fem', 'Real Madrid Fem']</t>
+    <t>['Tenerife', 'Real Madrid Fem', 'Sevilla FC Fem']</t>
+  </si>
+  <si>
+    <t>['Alhama ElPozo', 'Levante Fem', 'Real Madrid Fem', 'Tenerife', 'AtlÃ©tico Fem']</t>
+  </si>
+  <si>
+    <t>['Barcelona Fem', 'Real Sociedad', 'Sevilla FC Fem', 'AtlÃ©tico Fem', 'Real Madrid Fem']</t>
   </si>
   <si>
     <t>['Barcelona Fem', 'Valencia Fem', 'Levante Fem']</t>
@@ -309,25 +312,25 @@
     <t>['Valencia Fem', 'Sevilla FC Fem', 'Madrid CFF Fem']</t>
   </si>
   <si>
+    <t>['Real Madrid Fem', 'Alhama ElPozo', 'Madrid CFF Fem', 'Barcelona Fem', 'Valencia Fem']</t>
+  </si>
+  <si>
     <t>['Levante Fem']</t>
   </si>
   <si>
-    <t>['Alhama ElPozo', 'Madrid CFF Fem', 'Barcelona Fem', 'Valencia Fem']</t>
-  </si>
-  <si>
-    <t>['Real Madrid Fem', 'Villarreal', 'Levante Fem', 'Barcelona Fem']</t>
-  </si>
-  <si>
-    <t>['Madrid CFF Fem', 'Sevilla FC Fem']</t>
+    <t>['Levante Planas', 'Real Madrid Fem', 'Villarreal', 'Levante Fem', 'Barcelona Fem']</t>
+  </si>
+  <si>
+    <t>['Villarreal', 'Madrid CFF Fem', 'Sevilla FC Fem']</t>
   </si>
   <si>
     <t>['AtlÃ©tico Fem', 'Real Sociedad']</t>
   </si>
   <si>
+    <t>['AtlÃ©tico Fem']</t>
+  </si>
+  <si>
     <t>['Madrid CFF Fem']</t>
-  </si>
-  <si>
-    <t>['AtlÃ©tico Fem']</t>
   </si>
   <si>
     <t>['Alhama ElPozo']</t>
@@ -477,7 +480,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -492,16 +495,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.25</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -566,10 +569,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -584,16 +587,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.75</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,10 +750,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -765,16 +768,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.75</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.25</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -839,10 +842,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -857,10 +860,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.75</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2</c:v>
@@ -1020,10 +1023,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -1032,22 +1035,22 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.25</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1115,7 +1118,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1130,16 +1133,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,7 +1296,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -1311,13 +1314,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.25</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2</c:v>
@@ -1385,10 +1388,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -1403,13 +1406,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2</c:v>
@@ -1566,10 +1569,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -1584,13 +1587,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1658,10 +1661,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6</c:v>
@@ -1676,13 +1679,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1839,7 +1842,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1857,13 +1860,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.25</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1931,13 +1934,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1949,16 +1952,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2112,31 +2115,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2204,7 +2207,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -2222,13 +2225,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.25</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2385,13 +2388,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2403,13 +2406,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.75</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5</c:v>
@@ -2480,7 +2483,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -2495,16 +2498,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.25</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2724,7 +2727,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2742,13 +2745,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.25</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2882,10 +2885,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>6</c:v>
@@ -2900,13 +2903,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -3040,7 +3043,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -3058,13 +3061,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.25</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -3198,10 +3201,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3</c:v>
@@ -3216,10 +3219,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.75</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2</c:v>
@@ -3356,10 +3359,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3</c:v>
@@ -3368,22 +3371,22 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.5</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.25</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3514,7 +3517,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10</c:v>
@@ -3532,13 +3535,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.25</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2</c:v>
@@ -3657,7 +3660,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>30</c:v>
@@ -3672,34 +3675,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.75</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.25</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3815,7 +3818,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>30</c:v>
@@ -3830,34 +3833,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3988,10 +3991,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2</c:v>
@@ -4006,13 +4009,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2</c:v>
@@ -4146,10 +4149,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -4164,16 +4167,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.75</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4307,7 +4310,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -4322,16 +4325,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.25</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4462,13 +4465,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -4480,13 +4483,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.75</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>5</c:v>
@@ -4620,13 +4623,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -4638,16 +4641,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4763,10 +4766,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4778,34 +4781,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.75</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4921,10 +4924,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4936,34 +4939,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.25</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5097,7 +5100,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -5112,16 +5115,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5859,7 +5862,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -5874,16 +5877,16 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
-        <v>2.25</v>
+        <v>2.4</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5891,10 +5894,10 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5909,16 +5912,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -5978,10 +5981,10 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -5996,16 +5999,16 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="I2">
-        <v>2.25</v>
+        <v>2.2</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -6013,10 +6016,10 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -6031,10 +6034,10 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -6100,10 +6103,10 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -6112,22 +6115,22 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="I2">
-        <v>1.25</v>
+        <v>1.8</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -6138,7 +6141,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -6153,16 +6156,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -6222,7 +6225,7 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -6240,13 +6243,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.25</v>
+        <v>1.4</v>
       </c>
       <c r="I2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K2">
         <v>2</v>
@@ -6257,10 +6260,10 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -6275,13 +6278,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -6344,10 +6347,10 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -6362,13 +6365,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -6379,10 +6382,10 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -6397,13 +6400,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -6466,7 +6469,7 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -6484,13 +6487,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>5.25</v>
+        <v>5.6</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -6501,13 +6504,13 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -6519,16 +6522,16 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="I3">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -6588,31 +6591,31 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -6623,7 +6626,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6641,13 +6644,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -6710,13 +6713,13 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -6728,13 +6731,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>5</v>
@@ -6748,7 +6751,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -6763,16 +6766,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6898,7 +6901,7 @@
         <v>86</v>
       </c>
       <c r="M2">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -6916,13 +6919,13 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>5.25</v>
+        <v>5.6</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
       <c r="U2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -6966,10 +6969,10 @@
         <v>86</v>
       </c>
       <c r="M3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O3">
         <v>6</v>
@@ -6984,13 +6987,13 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="U3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -7034,7 +7037,7 @@
         <v>86</v>
       </c>
       <c r="M4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -7052,13 +7055,13 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="T4">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="U4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -7099,13 +7102,13 @@
         <v>86</v>
       </c>
       <c r="L5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O5">
         <v>3</v>
@@ -7120,10 +7123,10 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="U5">
         <v>2</v>
@@ -7164,16 +7167,16 @@
         <v>81</v>
       </c>
       <c r="K6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O6">
         <v>3</v>
@@ -7182,22 +7185,22 @@
         <v>2</v>
       </c>
       <c r="Q6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="T6">
-        <v>1.25</v>
+        <v>1.8</v>
       </c>
       <c r="U6">
         <v>3</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -7232,13 +7235,13 @@
         <v>82</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
         <v>86</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N7">
         <v>10</v>
@@ -7256,13 +7259,13 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>1.25</v>
+        <v>1.4</v>
       </c>
       <c r="T7">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V7">
         <v>2</v>
@@ -7273,7 +7276,7 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>60</v>
@@ -7291,7 +7294,7 @@
         <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="I8" t="s">
         <v>69</v>
@@ -7300,40 +7303,40 @@
         <v>83</v>
       </c>
       <c r="K8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N8">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="O8">
         <v>4</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
       <c r="S8">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T8">
-        <v>2.25</v>
+        <v>0.6</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="V8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -7341,7 +7344,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>60</v>
@@ -7359,7 +7362,7 @@
         <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
         <v>69</v>
@@ -7368,40 +7371,40 @@
         <v>84</v>
       </c>
       <c r="K9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="T9">
-        <v>0.25</v>
+        <v>2.2</v>
       </c>
       <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
         <v>5</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -7436,16 +7439,16 @@
         <v>85</v>
       </c>
       <c r="K10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O10">
         <v>2</v>
@@ -7460,13 +7463,13 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V10">
         <v>2</v>
@@ -7504,16 +7507,16 @@
         <v>86</v>
       </c>
       <c r="K11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L11" t="s">
         <v>86</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -7528,16 +7531,16 @@
         <v>1</v>
       </c>
       <c r="S11">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="T11">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -7572,7 +7575,7 @@
         <v>86</v>
       </c>
       <c r="K12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L12" t="s">
         <v>86</v>
@@ -7581,7 +7584,7 @@
         <v>1</v>
       </c>
       <c r="N12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -7596,16 +7599,16 @@
         <v>1</v>
       </c>
       <c r="S12">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="T12">
-        <v>2.25</v>
+        <v>2.4</v>
       </c>
       <c r="U12">
         <v>0</v>
       </c>
       <c r="V12">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -7637,22 +7640,22 @@
         <v>73</v>
       </c>
       <c r="J13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <v>15</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -7664,13 +7667,13 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="T13">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13">
         <v>5</v>
@@ -7708,19 +7711,19 @@
         <v>87</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L14" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -7732,16 +7735,16 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="T14">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="U14">
         <v>1</v>
       </c>
       <c r="V14">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -7749,7 +7752,7 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -7767,49 +7770,49 @@
         <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
         <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L15" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="M15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N15">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="O15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0.4</v>
+      </c>
+      <c r="T15">
+        <v>3.4</v>
+      </c>
+      <c r="U15">
         <v>0</v>
       </c>
-      <c r="S15">
-        <v>0.75</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
       <c r="V15">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -7817,7 +7820,7 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
@@ -7835,49 +7838,49 @@
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="I16" t="s">
         <v>75</v>
       </c>
       <c r="J16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>5</v>
+      </c>
+      <c r="O16">
         <v>2</v>
-      </c>
-      <c r="N16">
-        <v>13</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
         <v>1</v>
       </c>
-      <c r="S16">
-        <v>0.5</v>
-      </c>
       <c r="T16">
-        <v>3.25</v>
+        <v>1</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V16">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -7912,7 +7915,7 @@
         <v>86</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L17" t="s">
         <v>86</v>
@@ -7921,7 +7924,7 @@
         <v>1</v>
       </c>
       <c r="N17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -7936,16 +7939,16 @@
         <v>1</v>
       </c>
       <c r="S17">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="T17">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="U17">
         <v>0</v>
       </c>
       <c r="V17">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>